<commit_message>
Minor updates based on validation
</commit_message>
<xml_diff>
--- a/curation/draft/cdisc_biomedical_concepts_r15_draft.xlsx
+++ b/curation/draft/cdisc_biomedical_concepts_r15_draft.xlsx
@@ -4340,7 +4340,7 @@
       </c>
       <c r="F48" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests;Hematology Tests;Blood Cell Counts</t>
+          <t>Laboratory Tests;Hematology Tests;Blood Cell Counts;Blood Cell Count Ratio Measurements</t>
         </is>
       </c>
       <c r="G48" s="20" t="inlineStr"/>
@@ -4383,7 +4383,7 @@
       <c r="E49" s="20" t="n"/>
       <c r="F49" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Body Measurements</t>
         </is>
       </c>
       <c r="G49" s="20" t="inlineStr">
@@ -4450,7 +4450,7 @@
       <c r="E50" s="20" t="n"/>
       <c r="F50" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Body Measurements</t>
         </is>
       </c>
       <c r="G50" s="20" t="inlineStr">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="F63" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G63" s="20" t="inlineStr">
@@ -5464,7 +5464,7 @@
       </c>
       <c r="F64" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G64" s="20" t="inlineStr">
@@ -5547,7 +5547,7 @@
       </c>
       <c r="F65" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G65" s="20" t="inlineStr">
@@ -5634,7 +5634,7 @@
       </c>
       <c r="F66" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G66" s="20" t="inlineStr">
@@ -5717,7 +5717,7 @@
       </c>
       <c r="F67" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G67" s="20" t="inlineStr">
@@ -5804,7 +5804,7 @@
       </c>
       <c r="F68" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G68" s="20" t="inlineStr">
@@ -5891,7 +5891,7 @@
       </c>
       <c r="F69" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G69" s="20" t="inlineStr">
@@ -12548,7 +12548,7 @@
       <c r="E160" s="20" t="n"/>
       <c r="F160" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests;HematologyTests;Protein or Enzyme Type Measurements;Prothrombin Measurements;Coagulation Study</t>
+          <t>Laboratory Tests;Chemistry Tests;Protein or Enzyme Type Measurements;Prothrombin Measurements;Coagulation Study</t>
         </is>
       </c>
       <c r="G160" s="20" t="inlineStr">
@@ -12599,7 +12599,7 @@
       </c>
       <c r="F161" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests;Hematology Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
+          <t>Laboratory Tests;Chemistry Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
         </is>
       </c>
       <c r="G161" s="20" t="inlineStr">
@@ -12674,7 +12674,7 @@
       </c>
       <c r="F162" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests;Hematology Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
+          <t>Laboratory Tests;Chemistry Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
         </is>
       </c>
       <c r="G162" s="20" t="inlineStr">
@@ -12745,7 +12745,7 @@
       </c>
       <c r="F163" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests;Hematology Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
+          <t>Laboratory Tests;Chemistry Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
         </is>
       </c>
       <c r="G163" s="20" t="inlineStr">
@@ -12816,7 +12816,7 @@
       </c>
       <c r="F164" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests;Hematology Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
+          <t>Laboratory Tests;Chemistry Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
         </is>
       </c>
       <c r="G164" s="20" t="inlineStr">
@@ -12891,7 +12891,7 @@
       </c>
       <c r="F165" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests;Hematology Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
+          <t>Laboratory Tests;Chemistry Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
         </is>
       </c>
       <c r="G165" s="20" t="inlineStr">
@@ -15456,7 +15456,7 @@
       </c>
       <c r="F200" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G200" s="20" t="inlineStr">
@@ -15543,7 +15543,7 @@
       </c>
       <c r="F201" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G201" s="20" t="inlineStr">
@@ -15630,7 +15630,7 @@
       </c>
       <c r="F202" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G202" s="20" t="inlineStr">
@@ -15713,7 +15713,7 @@
       </c>
       <c r="F203" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G203" s="20" t="inlineStr">
@@ -15800,7 +15800,7 @@
       </c>
       <c r="F204" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G204" s="20" t="inlineStr">
@@ -15887,7 +15887,7 @@
       </c>
       <c r="F205" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G205" s="20" t="inlineStr">
@@ -15970,7 +15970,7 @@
       </c>
       <c r="F206" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="G206" s="20" t="inlineStr">
@@ -17158,7 +17158,7 @@
       <c r="E222" s="20" t="n"/>
       <c r="F222" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Body Measurements</t>
         </is>
       </c>
       <c r="G222" s="20" t="inlineStr">
@@ -17237,7 +17237,7 @@
       <c r="E223" s="20" t="n"/>
       <c r="F223" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Body Measurements</t>
         </is>
       </c>
       <c r="G223" s="20" t="inlineStr">
@@ -17320,7 +17320,7 @@
       <c r="E224" s="20" t="n"/>
       <c r="F224" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Body Measurements</t>
         </is>
       </c>
       <c r="G224" s="20" t="inlineStr">
@@ -17403,7 +17403,7 @@
       <c r="E225" s="20" t="n"/>
       <c r="F225" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Body Measurements</t>
         </is>
       </c>
       <c r="G225" s="20" t="inlineStr">
@@ -18120,7 +18120,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A54"/>
+  <dimension ref="A1:A56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -18197,313 +18197,327 @@
     <row r="10">
       <c r="A10" s="21" t="inlineStr">
         <is>
-          <t>Blood Cell Counts</t>
+          <t>Blood Cell Count Ratio Measurements</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="21" t="inlineStr">
         <is>
-          <t>Blood Protein Measurements</t>
+          <t>Blood Cell Counts</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="21" t="inlineStr">
         <is>
-          <t>COVID-19 Tests</t>
+          <t>Blood Pressure</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="21" t="inlineStr">
         <is>
-          <t>Chemistry Tests</t>
+          <t>Blood Protein Measurements</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="21" t="inlineStr">
         <is>
-          <t>Choriogonadotropin Measurements</t>
+          <t>Body Measurements</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="21" t="inlineStr">
         <is>
-          <t>Clinical Trial Attribute</t>
+          <t>COVID-19 Tests</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="21" t="inlineStr">
         <is>
-          <t>Clinical or Research Assessment Classification</t>
+          <t>Chemistry Tests</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="21" t="inlineStr">
         <is>
-          <t>Coagulation Study</t>
+          <t>Choriogonadotropin Measurements</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="21" t="inlineStr">
         <is>
-          <t>Coombs Tests</t>
+          <t>Clinical Trial Attribute</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="21" t="inlineStr">
         <is>
-          <t>DILI</t>
+          <t>Clinical or Research Assessment Classification</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="21" t="inlineStr">
         <is>
-          <t>Drug-Induced Liver Injury</t>
+          <t>Coagulation Study</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="21" t="inlineStr">
         <is>
-          <t>Events</t>
+          <t>Coombs Tests</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="21" t="inlineStr">
         <is>
-          <t>Factor III Measurements</t>
+          <t>DILI</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="21" t="inlineStr">
         <is>
-          <t>Gram Negative Bacteria Measurements</t>
+          <t>Drug-Induced Liver Injury</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="21" t="inlineStr">
         <is>
-          <t>HCG Measurements</t>
+          <t>Events</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="21" t="inlineStr">
         <is>
-          <t>Hematology Tests</t>
+          <t>Factor III Measurements</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="21" t="inlineStr">
         <is>
-          <t>HematologyTests</t>
+          <t>Gram Negative Bacteria Measurements</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="21" t="inlineStr">
         <is>
-          <t>Hormone Measurements</t>
+          <t>HCG Measurements</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="21" t="inlineStr">
         <is>
-          <t>Immunogenicity Specimen Assessments</t>
+          <t>Hematology Tests</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="21" t="inlineStr">
         <is>
-          <t>Immunoglobulin G Measurements</t>
+          <t>Hormone Measurements</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="21" t="inlineStr">
         <is>
-          <t>Immunohematology Tests</t>
+          <t>Immunogenicity Specimen Assessments</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="21" t="inlineStr">
         <is>
-          <t>Immunology Tests</t>
+          <t>Immunoglobulin G Measurements</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests</t>
+          <t>Immunohematology Tests</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="21" t="inlineStr">
         <is>
-          <t>Liver Function Tests</t>
+          <t>Immunology Tests</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="21" t="inlineStr">
         <is>
-          <t>MVAI</t>
+          <t>Laboratory Tests</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="21" t="inlineStr">
         <is>
-          <t>MVAI1</t>
+          <t>Liver Function Tests</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="21" t="inlineStr">
         <is>
-          <t>Medical Conditions</t>
+          <t>MVAI</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="21" t="inlineStr">
         <is>
-          <t>Medical History Events</t>
+          <t>MVAI1</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="21" t="inlineStr">
         <is>
-          <t>Microbial-induced Antibody Measurement</t>
+          <t>Medical Conditions</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="21" t="inlineStr">
         <is>
-          <t>Microbiology Tests</t>
+          <t>Medical History Events</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="21" t="inlineStr">
         <is>
-          <t>Modified Van Assche Index Clinical Classification</t>
+          <t>Microbial-induced Antibody Measurement</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="21" t="inlineStr">
         <is>
-          <t>Modified Van Assche Index Clinical Classification Question</t>
+          <t>Microbiology Tests</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="21" t="inlineStr">
         <is>
-          <t>Presenting Conditions</t>
+          <t>Modified Van Assche Index Clinical Classification</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="21" t="inlineStr">
         <is>
-          <t>Protein or Enzyme Type Measurements</t>
+          <t>Modified Van Assche Index Clinical Classification Question</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="21" t="inlineStr">
         <is>
-          <t>Prothrombin Activity Measurements</t>
+          <t>Presenting Conditions</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="21" t="inlineStr">
         <is>
-          <t>Prothrombin Measurements</t>
+          <t>Protein or Enzyme Type Measurements</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="21" t="inlineStr">
         <is>
-          <t>QRS</t>
+          <t>Prothrombin Activity Measurements</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="21" t="inlineStr">
         <is>
-          <t>QRS Instrument Questions</t>
+          <t>Prothrombin Measurements</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="21" t="inlineStr">
         <is>
-          <t>Reported Events</t>
+          <t>QRS</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="21" t="inlineStr">
         <is>
-          <t>SARS-CoV-2 Tests</t>
+          <t>QRS Instrument Questions</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="21" t="inlineStr">
         <is>
-          <t>Serology Tests</t>
+          <t>Reported Events</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="21" t="inlineStr">
         <is>
-          <t>Trial Summary</t>
+          <t>SARS-CoV-2 Tests</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="21" t="inlineStr">
         <is>
-          <t>Troponin Measurements</t>
+          <t>Serology Tests</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="21" t="inlineStr">
         <is>
-          <t>Virology Tests</t>
+          <t>Trial Summary</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="21" t="inlineStr">
+        <is>
+          <t>Troponin Measurements</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="21" t="inlineStr">
+        <is>
+          <t>Virology Tests</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="21" t="inlineStr">
         <is>
           <t>Vital Signs</t>
         </is>
@@ -18875,7 +18889,7 @@
       </c>
       <c r="E7" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests;Hematology Tests;Blood Cell Counts</t>
+          <t>Laboratory Tests;Hematology Tests;Blood Cell Counts;Blood Cell Count Ratio Measurements</t>
         </is>
       </c>
       <c r="F7" s="20" t="inlineStr"/>
@@ -18916,7 +18930,7 @@
       <c r="D8" s="20" t="inlineStr"/>
       <c r="E8" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Body Measurements</t>
         </is>
       </c>
       <c r="F8" s="20" t="inlineStr">
@@ -19177,7 +19191,7 @@
       </c>
       <c r="E13" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="F13" s="20" t="inlineStr">
@@ -20262,7 +20276,7 @@
       <c r="D34" s="20" t="inlineStr"/>
       <c r="E34" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests;HematologyTests;Protein or Enzyme Type Measurements;Prothrombin Measurements;Coagulation Study</t>
+          <t>Laboratory Tests;Chemistry Tests;Protein or Enzyme Type Measurements;Prothrombin Measurements;Coagulation Study</t>
         </is>
       </c>
       <c r="F34" s="20" t="inlineStr">
@@ -20311,7 +20325,7 @@
       </c>
       <c r="E35" s="21" t="inlineStr">
         <is>
-          <t>Laboratory Tests;Hematology Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
+          <t>Laboratory Tests;Chemistry Tests;Coagulation Study;Prothrombin Activity Measurements;Drug-Induced Liver Injury;DILI</t>
         </is>
       </c>
       <c r="F35" s="20" t="inlineStr">
@@ -20670,7 +20684,7 @@
       </c>
       <c r="E42" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Blood Pressure</t>
         </is>
       </c>
       <c r="F42" s="20" t="inlineStr">
@@ -20927,7 +20941,7 @@
       <c r="D47" s="20" t="inlineStr"/>
       <c r="E47" s="21" t="inlineStr">
         <is>
-          <t>Vital Signs</t>
+          <t>Vital Signs;Body Measurements</t>
         </is>
       </c>
       <c r="F47" s="20" t="inlineStr">

</xml_diff>